<commit_message>
Initial commit with Flask-based voice cloning app
</commit_message>
<xml_diff>
--- a/User_Data.xlsx
+++ b/User_Data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -642,6 +642,227 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>da0cb5dd-123d-4b56-b46d-f6973aca7c00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-03-d 21:12:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>dd4e5bd3-76a0-4e9e-866b-5915b554b789</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-03-d 21:12:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>c23811a0-d62c-4e4b-8cf5-840c9f527812</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-03-d 21:12:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Nguyen</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>d89c668a-a383-4f5d-9a6f-dc9a4313989b</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-03-d 15:54:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PHONG_OLD</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>63c2e3ba-ae2c-4ff7-a47f-9476fefddde5</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-03-d 15:56:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>a03726e7-a734-41ae-9f7e-da5b7246a331</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-03-d 15:58:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>598fec19-ac64-4230-92f0-63cd35d531e0</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:03:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3f358249-458d-4d40-a7ad-36127ca0a8e8</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:13:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>80a11c55-9172-4fd3-9ba1-ef5755a2db80</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:25:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5081cb67-6626-4fb4-b464-1ea38cc43d65</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:30:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PHONG_OLD</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>e8d307cd-ff42-4a49-a548-1b581edc8318</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:34:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>5976e3ea-2dd9-49d2-9ccf-efcff2d56f06</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:36:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>f107d882-0baf-44e0-b09f-5ad7a7fce4c7</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-03-d 16:39:45</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>